<commit_message>
fix bug and run examples notebook
</commit_message>
<xml_diff>
--- a/example/withdrawals.xlsx
+++ b/example/withdrawals.xlsx
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -441,7 +441,7 @@
         <v>44827</v>
       </c>
       <c r="C3">
-        <v>2324.07</v>
+        <v>2322.07</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -455,7 +455,7 @@
         <v>44827</v>
       </c>
       <c r="C4">
-        <v>934.41</v>
+        <v>936.41</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -525,7 +525,7 @@
         <v>44879</v>
       </c>
       <c r="C9">
-        <v>47.62</v>
+        <v>43.62</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>

</xml_diff>